<commit_message>
More upgrades in cap 09
</commit_message>
<xml_diff>
--- a/Capitulo-09/problema_do_roubo.xlsx
+++ b/Capitulo-09/problema_do_roubo.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Meus Documentos\Cursos\Técnico em Informática - SENAC\UC-03_Desenvolvimento\Tecnologias\Python\entendendo_algoritmos\Capitulo-09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Meus Documentos\Cursos\Técnico em Informática - SENAC\UC-03_Desenvolvimento\Tecnologias\Python\book-entendendo_algoritmos\Capitulo-09\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Programação Diânimca" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>1 KG</t>
   </si>
@@ -50,28 +50,124 @@
     <t>Programação Dinâmica</t>
   </si>
   <si>
-    <t>VIOLAO 1KG $ 1500</t>
-  </si>
-  <si>
-    <t>RADIO 4KG $ 3000</t>
-  </si>
-  <si>
-    <t>NOTEBOOK 3KG $ 2000</t>
-  </si>
-  <si>
-    <t>* IPHONE 1KG R$ 2000</t>
-  </si>
-  <si>
     <t>IPHONE</t>
   </si>
   <si>
-    <t>ITEM | PESO | VALOR</t>
-  </si>
-  <si>
-    <t>* MP3 1KG R$ 1000</t>
-  </si>
-  <si>
     <t>MP3</t>
+  </si>
+  <si>
+    <t>Westminster</t>
+  </si>
+  <si>
+    <t>Teatro the Globe</t>
+  </si>
+  <si>
+    <t>Galeria Nacional</t>
+  </si>
+  <si>
+    <t>Museu Britânico</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>0,5 DIA</t>
+  </si>
+  <si>
+    <t>1 DIA</t>
+  </si>
+  <si>
+    <t>1,5 DIA</t>
+  </si>
+  <si>
+    <t>2 DIA</t>
+  </si>
+  <si>
+    <t>CASACO</t>
+  </si>
+  <si>
+    <t>ÁGUA</t>
+  </si>
+  <si>
+    <t>LIVRO</t>
+  </si>
+  <si>
+    <t>COMIDA</t>
+  </si>
+  <si>
+    <t>CÂMERA</t>
+  </si>
+  <si>
+    <t>5 KG</t>
+  </si>
+  <si>
+    <t>6 KG</t>
+  </si>
+  <si>
+    <t>PESO</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>* IPHONE</t>
+  </si>
+  <si>
+    <t>* MP3</t>
+  </si>
+  <si>
+    <t>TEMPO</t>
+  </si>
+  <si>
+    <t>RANKING</t>
+  </si>
+  <si>
+    <t>LUGAR</t>
+  </si>
+  <si>
+    <t>ABADIA DE WESTMINSTER</t>
+  </si>
+  <si>
+    <t>TEATRO THE GLOBE</t>
+  </si>
+  <si>
+    <t>GALERIA NACIONAR</t>
+  </si>
+  <si>
+    <t>MUSEU BRITÂNICO</t>
+  </si>
+  <si>
+    <t>CATEDRAL DE SÃO PAULO</t>
+  </si>
+  <si>
+    <t>RELEVÂNCIA</t>
+  </si>
+  <si>
+    <t>Programação dinâmica na prática</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Maior substring comum</t>
   </si>
 </sst>
 </file>
@@ -81,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,7 +194,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -113,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -144,17 +247,26 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -165,9 +277,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -178,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,19 +297,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -209,22 +306,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -542,59 +645,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F6:N15"/>
+  <dimension ref="F6:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="L6" s="8" t="s">
+    <row r="6" spans="6:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="6:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="M6" s="10"/>
+      <c r="R6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="10"/>
+      <c r="U6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="V6" s="10"/>
+    </row>
+    <row r="7" spans="6:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="11"/>
+      <c r="M7" s="12"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="12"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="12"/>
+    </row>
+    <row r="8" spans="6:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="6:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J9" s="1"/>
-      <c r="K9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6" t="s">
+      <c r="K9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="J10" s="6" t="s">
+      <c r="R9" s="13"/>
+      <c r="S9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="6:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1500</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K10" s="2">
@@ -609,14 +749,36 @@
       <c r="N10" s="2">
         <v>1500</v>
       </c>
-    </row>
-    <row r="11" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="J11" s="6" t="s">
+      <c r="R10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+      <c r="T10" s="14">
+        <v>0</v>
+      </c>
+      <c r="U10" s="14">
+        <v>0</v>
+      </c>
+      <c r="V10" s="14">
+        <v>0</v>
+      </c>
+      <c r="W10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="6:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K11" s="2">
@@ -631,14 +793,36 @@
       <c r="N11" s="2">
         <v>3000</v>
       </c>
-    </row>
-    <row r="12" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F12" s="4"/>
-      <c r="G12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="J12" s="6" t="s">
+      <c r="R11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="14">
+        <v>0</v>
+      </c>
+      <c r="T11" s="14">
+        <v>1</v>
+      </c>
+      <c r="U11" s="14">
+        <v>0</v>
+      </c>
+      <c r="V11" s="14">
+        <v>0</v>
+      </c>
+      <c r="W11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="6:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="K12" s="2">
@@ -653,10 +837,37 @@
       <c r="N12" s="2">
         <v>3500</v>
       </c>
-    </row>
-    <row r="13" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="J13" s="7" t="s">
-        <v>12</v>
+      <c r="R12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S12" s="14">
+        <v>0</v>
+      </c>
+      <c r="T12" s="14">
+        <v>0</v>
+      </c>
+      <c r="U12" s="14">
+        <v>2</v>
+      </c>
+      <c r="V12" s="14">
+        <v>0</v>
+      </c>
+      <c r="W12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="6:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="K13" s="3">
         <v>2000</v>
@@ -670,15 +881,37 @@
       <c r="N13" s="3">
         <v>4000</v>
       </c>
-    </row>
-    <row r="14" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F14" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17"/>
-      <c r="J14" s="7" t="s">
-        <v>15</v>
+      <c r="R13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="S13" s="14">
+        <v>0</v>
+      </c>
+      <c r="T13" s="14">
+        <v>0</v>
+      </c>
+      <c r="U13" s="14">
+        <v>0</v>
+      </c>
+      <c r="V13" s="14">
+        <v>3</v>
+      </c>
+      <c r="W13" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="6:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="K14" s="3">
         <v>2000</v>
@@ -693,21 +926,357 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="15" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F15" s="10" t="s">
+    <row r="16" spans="6:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="5">
+        <v>7</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="5">
+        <v>7</v>
+      </c>
+      <c r="L18" s="5">
+        <v>7</v>
+      </c>
+      <c r="M18" s="5">
+        <v>7</v>
+      </c>
+      <c r="N18" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="5">
+        <v>6</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="5">
+        <v>7</v>
+      </c>
+      <c r="L19" s="5">
+        <v>13</v>
+      </c>
+      <c r="M19" s="5">
+        <v>13</v>
+      </c>
+      <c r="N19" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="5">
+        <v>9</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="5">
+        <v>7</v>
+      </c>
+      <c r="L20" s="5">
+        <v>13</v>
+      </c>
+      <c r="M20" s="5">
+        <v>16</v>
+      </c>
+      <c r="N20" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="5">
+        <v>9</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="5">
+        <v>7</v>
+      </c>
+      <c r="L21" s="5">
+        <v>13</v>
+      </c>
+      <c r="M21" s="5">
+        <v>16</v>
+      </c>
+      <c r="N21" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="5">
+        <v>8</v>
+      </c>
+      <c r="J22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="K22" s="5">
+        <v>8</v>
+      </c>
+      <c r="L22" s="5">
+        <v>15</v>
+      </c>
+      <c r="M22" s="5">
+        <v>21</v>
+      </c>
+      <c r="N22" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K25" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="5">
+        <v>10</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5">
+        <v>0</v>
+      </c>
+      <c r="M26" s="5">
+        <v>10</v>
+      </c>
+      <c r="N26" s="5">
+        <v>10</v>
+      </c>
+      <c r="O26" s="5">
+        <v>10</v>
+      </c>
+      <c r="P26" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6">
+        <v>3</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="5">
+        <v>3</v>
+      </c>
+      <c r="L27" s="5">
+        <v>3</v>
+      </c>
+      <c r="M27" s="5">
+        <v>10</v>
+      </c>
+      <c r="N27" s="5">
+        <v>13</v>
+      </c>
+      <c r="O27" s="5">
+        <v>13</v>
+      </c>
+      <c r="P27" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="6">
+        <v>9</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="5">
+        <v>3</v>
+      </c>
+      <c r="L28" s="5">
+        <v>9</v>
+      </c>
+      <c r="M28" s="5">
+        <v>10</v>
+      </c>
+      <c r="N28" s="5">
+        <v>13</v>
+      </c>
+      <c r="O28" s="5">
+        <v>19</v>
+      </c>
+      <c r="P28" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="6">
+        <v>5</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="5">
+        <v>3</v>
+      </c>
+      <c r="L29" s="5">
+        <v>9</v>
+      </c>
+      <c r="M29" s="5">
+        <v>12</v>
+      </c>
+      <c r="N29" s="5">
+        <v>14</v>
+      </c>
+      <c r="O29" s="5">
+        <v>19</v>
+      </c>
+      <c r="P29" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
+        <v>6</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="5">
+        <v>6</v>
+      </c>
+      <c r="L30" s="5">
+        <v>9</v>
+      </c>
+      <c r="M30" s="5">
+        <v>15</v>
+      </c>
+      <c r="N30" s="5">
+        <v>16</v>
+      </c>
+      <c r="O30" s="5">
+        <v>20</v>
+      </c>
+      <c r="P30" s="5">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
+  <mergeCells count="3">
     <mergeCell ref="L6:M7"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="R6:S7"/>
+    <mergeCell ref="U6:V7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>